<commit_message>
Finalização dos exercícios da L1 de PLA
</commit_message>
<xml_diff>
--- a/Exercicios/Exercicios - L1 - PL.xlsx
+++ b/Exercicios/Exercicios - L1 - PL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhfer\Documents\Fatec\PLA 2025\Exercícios Resolvidos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Estudos\Cursos\Autodidata\Programação Linear\Exercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F2A39A-18B0-456A-9CE6-BA5616310D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F578FC6-6B78-432F-B0AD-59084B61964F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{B72F011D-5390-4C7B-A479-D289570F6EC7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{B72F011D-5390-4C7B-A479-D289570F6EC7}"/>
   </bookViews>
   <sheets>
     <sheet name="1) Fábrica" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="3) Criação Porcos" sheetId="4" r:id="rId3"/>
     <sheet name="4) Automóveis" sheetId="5" r:id="rId4"/>
     <sheet name="5) Fertilizantes" sheetId="6" r:id="rId5"/>
+    <sheet name="6) Azeitex" sheetId="7" r:id="rId6"/>
+    <sheet name="7) Empresa de Eletrônicos" sheetId="8" r:id="rId7"/>
+    <sheet name="8) Dpt. Marketing" sheetId="9" r:id="rId8"/>
+    <sheet name="9) Notas Aluno" sheetId="10" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'1) Fábrica'!$B$6:$C$6</definedName>
@@ -25,226 +29,412 @@
     <definedName name="solver_adj" localSheetId="2" hidden="1">'3) Criação Porcos'!$B$3:$C$3</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'4) Automóveis'!$B$3:$B$4</definedName>
     <definedName name="solver_adj" localSheetId="4" hidden="1">'5) Fertilizantes'!$E$3:$E$5</definedName>
+    <definedName name="solver_adj" localSheetId="5" hidden="1">'6) Azeitex'!$F$3:$F$6</definedName>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'7) Empresa de Eletrônicos'!$B$3:$B$4</definedName>
+    <definedName name="solver_adj" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$3:$B$5</definedName>
+    <definedName name="solver_adj" localSheetId="8" hidden="1">'9) Notas Aluno'!$B$3:$B$5</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="5" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="7" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="8" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_drv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'1) Fábrica'!$B$11</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$11</definedName>
     <definedName name="solver_lhs1" localSheetId="2" hidden="1">'3) Criação Porcos'!$B$3</definedName>
     <definedName name="solver_lhs1" localSheetId="3" hidden="1">'4) Automóveis'!$B$10</definedName>
     <definedName name="solver_lhs1" localSheetId="4" hidden="1">'5) Fertilizantes'!$E$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="5" hidden="1">'6) Azeitex'!$C$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'7) Empresa de Eletrônicos'!$B$3</definedName>
+    <definedName name="solver_lhs1" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$3</definedName>
+    <definedName name="solver_lhs1" localSheetId="8" hidden="1">'9) Notas Aluno'!$B$3</definedName>
+    <definedName name="solver_lhs10" localSheetId="5" hidden="1">'6) Azeitex'!$F$6</definedName>
+    <definedName name="solver_lhs11" localSheetId="5" hidden="1">'6) Azeitex'!$F$6</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'1) Fábrica'!$B$12</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$12</definedName>
     <definedName name="solver_lhs2" localSheetId="2" hidden="1">'3) Criação Porcos'!$C$3</definedName>
     <definedName name="solver_lhs2" localSheetId="3" hidden="1">'4) Automóveis'!$B$11</definedName>
     <definedName name="solver_lhs2" localSheetId="4" hidden="1">'5) Fertilizantes'!$E$3</definedName>
+    <definedName name="solver_lhs2" localSheetId="5" hidden="1">'6) Azeitex'!$D$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="6" hidden="1">'7) Empresa de Eletrônicos'!$B$3:$B$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="8" hidden="1">'9) Notas Aluno'!$B$4</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'1) Fábrica'!$B$6</definedName>
     <definedName name="solver_lhs3" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$6</definedName>
     <definedName name="solver_lhs3" localSheetId="2" hidden="1">'3) Criação Porcos'!$D$5</definedName>
     <definedName name="solver_lhs3" localSheetId="3" hidden="1">'4) Automóveis'!$B$12</definedName>
     <definedName name="solver_lhs3" localSheetId="4" hidden="1">'5) Fertilizantes'!$E$4</definedName>
+    <definedName name="solver_lhs3" localSheetId="5" hidden="1">'6) Azeitex'!$E$8</definedName>
+    <definedName name="solver_lhs3" localSheetId="6" hidden="1">'7) Empresa de Eletrônicos'!$B$4</definedName>
+    <definedName name="solver_lhs3" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$5</definedName>
+    <definedName name="solver_lhs3" localSheetId="8" hidden="1">'9) Notas Aluno'!$B$5</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'1) Fábrica'!$B$6</definedName>
     <definedName name="solver_lhs4" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$6</definedName>
     <definedName name="solver_lhs4" localSheetId="2" hidden="1">'3) Criação Porcos'!$D$6</definedName>
     <definedName name="solver_lhs4" localSheetId="3" hidden="1">'4) Automóveis'!$B$3</definedName>
     <definedName name="solver_lhs4" localSheetId="4" hidden="1">'5) Fertilizantes'!$E$5</definedName>
+    <definedName name="solver_lhs4" localSheetId="5" hidden="1">'6) Azeitex'!$F$3</definedName>
+    <definedName name="solver_lhs4" localSheetId="6" hidden="1">'7) Empresa de Eletrônicos'!$B$5</definedName>
+    <definedName name="solver_lhs4" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="8" hidden="1">'9) Notas Aluno'!$B$7</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'1) Fábrica'!$C$6</definedName>
     <definedName name="solver_lhs5" localSheetId="1" hidden="1">'2) Direção Marketing'!$C$6</definedName>
     <definedName name="solver_lhs5" localSheetId="2" hidden="1">'3) Criação Porcos'!$D$7</definedName>
     <definedName name="solver_lhs5" localSheetId="3" hidden="1">'4) Automóveis'!$B$3</definedName>
     <definedName name="solver_lhs5" localSheetId="4" hidden="1">'5) Fertilizantes'!$E$8</definedName>
+    <definedName name="solver_lhs5" localSheetId="5" hidden="1">'6) Azeitex'!$F$3</definedName>
+    <definedName name="solver_lhs5" localSheetId="6" hidden="1">'7) Empresa de Eletrônicos'!$D$5</definedName>
+    <definedName name="solver_lhs5" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$8</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'1) Fábrica'!$C$6</definedName>
     <definedName name="solver_lhs6" localSheetId="3" hidden="1">'4) Automóveis'!$B$4</definedName>
     <definedName name="solver_lhs6" localSheetId="4" hidden="1">'5) Fertilizantes'!$E$9</definedName>
+    <definedName name="solver_lhs6" localSheetId="5" hidden="1">'6) Azeitex'!$F$4</definedName>
+    <definedName name="solver_lhs6" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$9</definedName>
     <definedName name="solver_lhs7" localSheetId="3" hidden="1">'4) Automóveis'!$B$4</definedName>
+    <definedName name="solver_lhs7" localSheetId="5" hidden="1">'6) Azeitex'!$F$4</definedName>
     <definedName name="solver_lhs8" localSheetId="3" hidden="1">'4) Automóveis'!$B$9</definedName>
+    <definedName name="solver_lhs8" localSheetId="5" hidden="1">'6) Azeitex'!$F$5</definedName>
+    <definedName name="solver_lhs9" localSheetId="5" hidden="1">'6) Azeitex'!$F$5</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="5" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="7" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="8" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="5" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="7" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="8" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">6</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_num" localSheetId="3" hidden="1">8</definedName>
     <definedName name="solver_num" localSheetId="4" hidden="1">6</definedName>
+    <definedName name="solver_num" localSheetId="5" hidden="1">11</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="7" hidden="1">6</definedName>
+    <definedName name="solver_num" localSheetId="8" hidden="1">4</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'1) Fábrica'!$B$8</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$8</definedName>
     <definedName name="solver_opt" localSheetId="2" hidden="1">'3) Criação Porcos'!$D$8</definedName>
     <definedName name="solver_opt" localSheetId="3" hidden="1">'4) Automóveis'!$B$6</definedName>
     <definedName name="solver_opt" localSheetId="4" hidden="1">'5) Fertilizantes'!$B$14</definedName>
+    <definedName name="solver_opt" localSheetId="5" hidden="1">'6) Azeitex'!$B$12</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'7) Empresa de Eletrônicos'!$C$5</definedName>
+    <definedName name="solver_opt" localSheetId="7" hidden="1">'8) Dpt. Marketing'!$B$7</definedName>
+    <definedName name="solver_opt" localSheetId="8" hidden="1">'9) Notas Aluno'!$B$8</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="5" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="7" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="8" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rbv" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="8" hidden="1">3</definedName>
+    <definedName name="solver_rel10" localSheetId="5" hidden="1">4</definedName>
+    <definedName name="solver_rel11" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rel2" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="6" hidden="1">4</definedName>
+    <definedName name="solver_rel2" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_rel2" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="8" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="3" hidden="1">4</definedName>
     <definedName name="solver_rel4" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="5" hidden="1">4</definedName>
+    <definedName name="solver_rel4" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="3" hidden="1">4</definedName>
     <definedName name="solver_rel6" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="5" hidden="1">4</definedName>
+    <definedName name="solver_rel6" localSheetId="7" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="3" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rel8" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="5" hidden="1">4</definedName>
+    <definedName name="solver_rel9" localSheetId="5" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'1) Fábrica'!$B$13</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$13</definedName>
     <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="4" hidden="1">100000</definedName>
+    <definedName name="solver_rhs1" localSheetId="5" hidden="1">650</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_rhs1" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_rhs10" localSheetId="5" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs11" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'1) Fábrica'!$B$14</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$14</definedName>
     <definedName name="solver_rhs2" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="3" hidden="1">6750</definedName>
     <definedName name="solver_rhs2" localSheetId="4" hidden="1">5000</definedName>
+    <definedName name="solver_rhs2" localSheetId="5" hidden="1">700</definedName>
+    <definedName name="solver_rhs2" localSheetId="6" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs2" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">"número inteiro"</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">'2) Direção Marketing'!$B$15</definedName>
     <definedName name="solver_rhs3" localSheetId="2" hidden="1">200</definedName>
     <definedName name="solver_rhs3" localSheetId="3" hidden="1">4500</definedName>
     <definedName name="solver_rhs3" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="5" hidden="1">700</definedName>
+    <definedName name="solver_rhs3" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs4" localSheetId="2" hidden="1">150</definedName>
     <definedName name="solver_rhs4" localSheetId="3" hidden="1">"número inteiro"</definedName>
     <definedName name="solver_rhs4" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="5" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs4" localSheetId="6" hidden="1">10</definedName>
+    <definedName name="solver_rhs4" localSheetId="7" hidden="1">10</definedName>
+    <definedName name="solver_rhs4" localSheetId="8" hidden="1">100</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">"número inteiro"</definedName>
     <definedName name="solver_rhs5" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="2" hidden="1">210</definedName>
     <definedName name="solver_rhs5" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="4" hidden="1">15000</definedName>
+    <definedName name="solver_rhs5" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="6" hidden="1">6000</definedName>
+    <definedName name="solver_rhs5" localSheetId="7" hidden="1">30</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs6" localSheetId="3" hidden="1">"número inteiro"</definedName>
     <definedName name="solver_rhs6" localSheetId="4" hidden="1">12000</definedName>
+    <definedName name="solver_rhs6" localSheetId="5" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs6" localSheetId="7" hidden="1">30</definedName>
     <definedName name="solver_rhs7" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_rhs7" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rhs8" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rhs8" localSheetId="5" hidden="1">"número inteiro"</definedName>
+    <definedName name="solver_rhs9" localSheetId="5" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="8" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="5" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="7" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="8" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="5" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="7" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="8" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="5" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="7" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="8" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="5" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="7" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="8" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="5" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="7" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="8" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="5" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="7" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -267,7 +457,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="95">
   <si>
     <t>Produto</t>
   </si>
@@ -435,18 +625,136 @@
   </si>
   <si>
     <t>Produção mínima</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Margem</t>
+  </si>
+  <si>
+    <t>Prensagem (h)</t>
+  </si>
+  <si>
+    <t>Refinação (h)</t>
+  </si>
+  <si>
+    <t>Embalamento (h)</t>
+  </si>
+  <si>
+    <t>Produção (x)</t>
+  </si>
+  <si>
+    <t>Total gasto:</t>
+  </si>
+  <si>
+    <t>Limite:</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>Produção de Azeites</t>
+  </si>
+  <si>
+    <t>Variáveis</t>
+  </si>
+  <si>
+    <t>Valor Gerado</t>
+  </si>
+  <si>
+    <t>Custo Salarial</t>
+  </si>
+  <si>
+    <t>Trabalhadores experientes</t>
+  </si>
+  <si>
+    <t>Trabalhadores menos experientes</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Empresa de Eletrônicos</t>
+  </si>
+  <si>
+    <t>Programa Institucional</t>
+  </si>
+  <si>
+    <t>Departamento de Marketing</t>
+  </si>
+  <si>
+    <t>Investimentos</t>
+  </si>
+  <si>
+    <t>Valor ($ 1.000)</t>
+  </si>
+  <si>
+    <t>Aumento P1</t>
+  </si>
+  <si>
+    <t>Aumento P2</t>
+  </si>
+  <si>
+    <t>Divulgação Direta P1</t>
+  </si>
+  <si>
+    <t>Divulgação Direta P2</t>
+  </si>
+  <si>
+    <t>Total investido:</t>
+  </si>
+  <si>
+    <t>Aumento total P1 (%)</t>
+  </si>
+  <si>
+    <t>Aumento total P2 (%)</t>
+  </si>
+  <si>
+    <t>Valor total ($):</t>
+  </si>
+  <si>
+    <t>Disciplina</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>Pontos Ganhos</t>
+  </si>
+  <si>
+    <t>Nota final</t>
+  </si>
+  <si>
+    <t>Total de horas:</t>
+  </si>
+  <si>
+    <t>Soma total de notas:</t>
+  </si>
+  <si>
+    <t>Notas Aluno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,6 +773,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,7 +863,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,6 +896,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -598,24 +933,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -958,20 +1275,20 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -982,7 +1299,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -993,7 +1310,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1004,7 +1321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1026,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1035,19 +1352,19 @@
         <v>280</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
@@ -1056,7 +1373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
@@ -1065,7 +1382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1098,20 +1415,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="20.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -1133,7 +1450,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1144,7 +1461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>16</v>
       </c>
@@ -1155,7 +1472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
@@ -1166,7 +1483,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
@@ -1175,13 +1492,13 @@
         <v>8200</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1190,7 +1507,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
@@ -1199,7 +1516,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -1207,7 +1524,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -1215,7 +1532,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
@@ -1240,21 +1557,21 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="20.7109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="25.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="20.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
@@ -1265,7 +1582,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
@@ -1276,7 +1593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>33</v>
       </c>
@@ -1290,7 +1607,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -1305,7 +1622,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
@@ -1320,7 +1637,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
@@ -1335,7 +1652,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>28</v>
       </c>
@@ -1368,21 +1685,21 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" style="1" customWidth="1"/>
-    <col min="2" max="3" width="20.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="20.6640625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>42</v>
       </c>
@@ -1393,7 +1710,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
@@ -1404,7 +1721,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>40</v>
       </c>
@@ -1415,10 +1732,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" s="10"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -1428,13 +1745,13 @@
       </c>
       <c r="C6" s="10"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="11"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
@@ -1443,7 +1760,7 @@
         <v>0.99990476190476185</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>39</v>
       </c>
@@ -1452,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>44</v>
       </c>
@@ -1461,7 +1778,7 @@
         <v>6110</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>45</v>
       </c>
@@ -1483,43 +1800,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4BCAEB-6F7F-4508-B9E8-572E73ECC37B}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="123" zoomScaleNormal="123" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="5" width="20.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="5" width="20.6640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="11" t="s">
         <v>50</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1853,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -1553,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
@@ -1570,29 +1887,28 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="2">
         <v>15000</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="22" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="13" t="s">
         <v>54</v>
       </c>
       <c r="E8" s="2">
@@ -1600,15 +1916,15 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="19">
+      <c r="B9" s="2">
         <v>12000</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="22" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="13" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="2">
@@ -1616,15 +1932,15 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="12">
         <v>100000</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="13" t="s">
         <v>53</v>
       </c>
       <c r="E10" s="9">
@@ -1632,19 +1948,15 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
@@ -1659,5 +1971,525 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{241D8A67-3C68-4FDD-B92B-BBF49B540D85}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="16.44140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9">
+        <v>40</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="9">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="9">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="9">
+        <v>36</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1.25</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="2">
+        <f>(C3*F3)+(C4*F4)+(C5*F5)+(C6*F6)</f>
+        <v>582.5</v>
+      </c>
+      <c r="D8" s="2">
+        <f>(D3*F3)+(D4*F4)+(D5*F5)+(D6*F6)</f>
+        <v>699</v>
+      </c>
+      <c r="E8" s="2">
+        <f>(E3*F3)+(E4*F4)+(E5*F5)+(E6*F6)</f>
+        <v>699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="2">
+        <v>650</v>
+      </c>
+      <c r="D9" s="2">
+        <v>700</v>
+      </c>
+      <c r="E9" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="9">
+        <f>(B3*F3)+(B4*F4)+(B5*F5)+(B6*F6)</f>
+        <v>16776</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA50CBCD-4D7F-49DE-B0F9-BECD0CDF8712}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" style="15" customWidth="1"/>
+    <col min="2" max="4" width="18.6640625" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14">
+        <f>B3*2000</f>
+        <v>4000</v>
+      </c>
+      <c r="D3" s="14">
+        <f>B3*1000</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="14">
+        <v>5</v>
+      </c>
+      <c r="C4" s="14">
+        <f>B4*1800</f>
+        <v>9000</v>
+      </c>
+      <c r="D4" s="14">
+        <f>B4*800</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="14">
+        <f>SUM(B3:B4)</f>
+        <v>7</v>
+      </c>
+      <c r="C5" s="14">
+        <f t="shared" ref="C5:D5" si="0">SUM(C3:C4)</f>
+        <v>13000</v>
+      </c>
+      <c r="D5" s="14">
+        <f t="shared" si="0"/>
+        <v>6000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49A963C0-E107-4601-87FE-05AC6DD5CBD7}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.88671875" style="15" customWidth="1"/>
+    <col min="2" max="2" width="26" style="15" customWidth="1"/>
+    <col min="3" max="5" width="15" style="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="14">
+        <v>9.9999999999999893</v>
+      </c>
+      <c r="C3" s="14">
+        <v>3</v>
+      </c>
+      <c r="D3" s="14">
+        <v>3</v>
+      </c>
+      <c r="E3" s="16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="17">
+        <v>6.2172489379008798E-15</v>
+      </c>
+      <c r="C4" s="14">
+        <v>4</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2.2204460492503131E-15</v>
+      </c>
+      <c r="C5" s="14">
+        <v>0</v>
+      </c>
+      <c r="D5" s="14">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="14">
+        <f>SUM(B3:B5)</f>
+        <v>9.9999999999999982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="14">
+        <f>(3*B3)+(4*B4)</f>
+        <v>29.999999999999993</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="14">
+        <f>(3*B3)+(10*B5)</f>
+        <v>29.999999999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="14">
+        <f>1000*B7</f>
+        <v>9999.9999999999982</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1276F3D9-F935-47EF-8F0C-A9EBEDB3C110}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="15" customWidth="1"/>
+    <col min="2" max="4" width="14.6640625" style="15" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14">
+        <f>B3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="14">
+        <f>6+B3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="14">
+        <v>0</v>
+      </c>
+      <c r="C4" s="14">
+        <f>(2*B4)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="14">
+        <f>7+(2*B4)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="14">
+        <v>100</v>
+      </c>
+      <c r="C5" s="14">
+        <f>(3*B5)</f>
+        <v>300</v>
+      </c>
+      <c r="D5" s="14">
+        <f>10+3*B5</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="14">
+        <f>SUM(B3:B5)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="14">
+        <f>SUM(D3:D5)</f>
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>